<commit_message>
Changes to Report Balance API: more descriptive; changes to fetching team and object for report
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Отчет Остатка.xlsx
+++ b/pkg/excels/templates/Отчет Остатка.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B39D9E2-16E8-4CD5-93F3-6ED67078E9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FD62D3-A7BB-4FEF-A1CC-86C8D2DFF10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +389,7 @@
     <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -414,8 +414,6 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>